<commit_message>
dendrometer key not completed
</commit_message>
<xml_diff>
--- a/R/01_rawdata/phenological_monitoring.xlsx
+++ b/R/01_rawdata/phenological_monitoring.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christophe_rouleau-desrochers/Documents/github/fuelinex/R/01_rawdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{861AF9C5-CFDE-794A-BC11-470A77344FA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA87412F-AA21-8344-840E-E1DFF79D7C34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17180" activeTab="1" xr2:uid="{185C83C0-866D-5047-837F-AA9A16B7FD6C}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17140" xr2:uid="{185C83C0-866D-5047-837F-AA9A16B7FD6C}"/>
   </bookViews>
   <sheets>
     <sheet name="metadata" sheetId="2" r:id="rId1"/>
@@ -2679,9 +2679,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2719,7 +2719,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2825,7 +2825,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2967,7 +2967,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2977,8 +2977,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36950948-9D01-2E4A-811C-B847B8E678B8}">
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView zoomScale="208" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" zoomScale="208" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3075,8 +3075,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F49363F8-6720-B149-85E7-6B9B7FC84DA7}">
   <dimension ref="A1:AG811"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="170" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView zoomScale="170" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>